<commit_message>
GUI building PYQT5 (experimentation)
</commit_message>
<xml_diff>
--- a/src/Department MI.xlsx
+++ b/src/Department MI.xlsx
@@ -2567,7 +2567,7 @@
       </c>
       <c r="H8" s="17" t="inlineStr">
         <is>
-          <t>TG, TD/ G1, S4, Mr Ablaoui H.</t>
+          <t>TG, TD/ G1, S3, Mr Ablaoui H.</t>
         </is>
       </c>
     </row>
@@ -2659,7 +2659,7 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>OAF 2, COUR/ section 1, C4, Mr S. M. Bahri</t>
+          <t>OAF 2, COUR/ section 1, S14, Mr S. M. Bahri</t>
         </is>
       </c>
       <c r="C17" s="29" t="inlineStr">
@@ -2669,7 +2669,7 @@
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>PROGQUAD, TD/ G1, S12, M. AMIR A.</t>
+          <t>PROGQUAD, TD/ G1, C3, M. AMIR A.</t>
         </is>
       </c>
       <c r="E17" s="17" t="inlineStr">
@@ -9722,17 +9722,17 @@
       </c>
       <c r="F8" s="17" t="inlineStr">
         <is>
-          <t>ANA4, TD/ G1, S15, Mme Limam</t>
+          <t>AC, TD/ G1, S2, Mlle Amina FERRAOUN</t>
         </is>
       </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>AC, TD/ G1, S14, Mlle Amina FERRAOUN</t>
+          <t>ANUM2, TD/ G1, S14, M. Belhamiti Omar</t>
         </is>
       </c>
       <c r="H8" s="17" t="inlineStr">
         <is>
-          <t>ANUM2, TD/ G1, S13, M. Belhamiti Omar</t>
+          <t>PROBA, TD/ G1, S13, M. Mohammedi Mustapha</t>
         </is>
       </c>
     </row>
@@ -9752,7 +9752,7 @@
       </c>
       <c r="F9" s="27" t="inlineStr">
         <is>
-          <t>ANUM2, TD/ G2, S2, M. Belhamiti Omar</t>
+          <t>ANA4, TD/ G2, S15, Mme Limam</t>
         </is>
       </c>
       <c r="G9" s="27" t="inlineStr">
@@ -9762,7 +9762,7 @@
       </c>
       <c r="H9" s="27" t="inlineStr">
         <is>
-          <t>ANA4, TD/ G2, S12, Mme Limam</t>
+          <t>ANUM2, TD/ G2, S12, M. Belhamiti Omar</t>
         </is>
       </c>
     </row>
@@ -9842,53 +9842,53 @@
           <t>Lundi</t>
         </is>
       </c>
-      <c r="B17" s="29" t="inlineStr">
+      <c r="B17" s="17" t="inlineStr">
+        <is>
+          <t>ANA4, TD/ G1, C2, Mme Limam</t>
+        </is>
+      </c>
+      <c r="C17" s="29" t="inlineStr">
         <is>
           <t>ALG4, COUR/ section 1, S16, M.Ould ali</t>
         </is>
       </c>
-      <c r="C17" s="29" t="inlineStr">
+      <c r="D17" s="29" t="inlineStr">
         <is>
           <t>AC, COUR/ section 1, S16, Mlle Amina FERRAOUN</t>
         </is>
       </c>
-      <c r="D17" s="17" t="inlineStr">
-        <is>
-          <t>PROBA, TD/ G1, C2, M. Mohammedi Mustapha</t>
-        </is>
-      </c>
       <c r="E17" s="17" t="inlineStr">
         <is>
-          <t>GÉOMÉ, TD/ G1, B4, Mme Bendahmane Hafida</t>
-        </is>
-      </c>
-      <c r="F17" s="17" t="n"/>
+          <t>GÉOMÉ, TD/ G1, B3, Mme Bendahmane Hafida</t>
+        </is>
+      </c>
+      <c r="F17" s="17" t="inlineStr">
+        <is>
+          <t>GÉOMÉ, TD/ G2, S1, Mme Bendahmane Hafida</t>
+        </is>
+      </c>
       <c r="G17" s="17" t="n"/>
       <c r="H17" s="17" t="n"/>
     </row>
     <row r="18" ht="21.75" customHeight="1" s="24">
       <c r="A18" s="30" t="n"/>
-      <c r="B18" s="31" t="n"/>
+      <c r="B18" s="27" t="inlineStr">
+        <is>
+          <t>PROBA, TD/ G2, C3, M. Mohammedi Mustapha</t>
+        </is>
+      </c>
       <c r="C18" s="31" t="n"/>
-      <c r="D18" s="27" t="inlineStr">
-        <is>
-          <t>GÉOMÉ, TD/ G2, C3, Mme Bendahmane Hafida</t>
-        </is>
-      </c>
-      <c r="E18" s="27" t="inlineStr">
-        <is>
-          <t>PROBA, TD/ G2, B3, M. Mohammedi Mustapha</t>
-        </is>
-      </c>
+      <c r="D18" s="31" t="n"/>
+      <c r="E18" s="27" t="n"/>
       <c r="F18" s="27" t="n"/>
       <c r="G18" s="27" t="n"/>
       <c r="H18" s="27" t="n"/>
     </row>
     <row r="19" ht="21.75" customHeight="1" s="24">
       <c r="A19" s="30" t="n"/>
-      <c r="B19" s="31" t="n"/>
+      <c r="B19" s="27" t="n"/>
       <c r="C19" s="31" t="n"/>
-      <c r="D19" s="27" t="n"/>
+      <c r="D19" s="31" t="n"/>
       <c r="E19" s="27" t="n"/>
       <c r="F19" s="27" t="n"/>
       <c r="G19" s="27" t="n"/>
@@ -9896,9 +9896,9 @@
     </row>
     <row r="20" ht="21.75" customHeight="1" s="24">
       <c r="A20" s="30" t="n"/>
-      <c r="B20" s="31" t="n"/>
+      <c r="B20" s="27" t="n"/>
       <c r="C20" s="31" t="n"/>
-      <c r="D20" s="27" t="n"/>
+      <c r="D20" s="31" t="n"/>
       <c r="E20" s="27" t="n"/>
       <c r="F20" s="27" t="n"/>
       <c r="G20" s="27" t="n"/>
@@ -9906,9 +9906,9 @@
     </row>
     <row r="21" ht="21.75" customHeight="1" s="24">
       <c r="A21" s="30" t="n"/>
-      <c r="B21" s="31" t="n"/>
+      <c r="B21" s="27" t="n"/>
       <c r="C21" s="31" t="n"/>
-      <c r="D21" s="27" t="n"/>
+      <c r="D21" s="31" t="n"/>
       <c r="E21" s="27" t="n"/>
       <c r="F21" s="27" t="n"/>
       <c r="G21" s="27" t="n"/>
@@ -9916,9 +9916,9 @@
     </row>
     <row r="22" ht="21.75" customHeight="1" s="24">
       <c r="A22" s="30" t="n"/>
-      <c r="B22" s="31" t="n"/>
+      <c r="B22" s="27" t="n"/>
       <c r="C22" s="31" t="n"/>
-      <c r="D22" s="27" t="n"/>
+      <c r="D22" s="31" t="n"/>
       <c r="E22" s="27" t="n"/>
       <c r="F22" s="27" t="n"/>
       <c r="G22" s="27" t="n"/>
@@ -9926,9 +9926,9 @@
     </row>
     <row r="23" ht="21.75" customHeight="1" s="24">
       <c r="A23" s="30" t="n"/>
-      <c r="B23" s="31" t="n"/>
+      <c r="B23" s="27" t="n"/>
       <c r="C23" s="31" t="n"/>
-      <c r="D23" s="27" t="n"/>
+      <c r="D23" s="31" t="n"/>
       <c r="E23" s="27" t="n"/>
       <c r="F23" s="27" t="n"/>
       <c r="G23" s="27" t="n"/>
@@ -9936,9 +9936,9 @@
     </row>
     <row r="24" ht="21.75" customHeight="1" s="24">
       <c r="A24" s="30" t="n"/>
-      <c r="B24" s="31" t="n"/>
+      <c r="B24" s="27" t="n"/>
       <c r="C24" s="31" t="n"/>
-      <c r="D24" s="27" t="n"/>
+      <c r="D24" s="31" t="n"/>
       <c r="E24" s="27" t="n"/>
       <c r="F24" s="27" t="n"/>
       <c r="G24" s="27" t="n"/>
@@ -9946,9 +9946,9 @@
     </row>
     <row r="25" ht="21.75" customHeight="1" s="24">
       <c r="A25" s="32" t="n"/>
-      <c r="B25" s="33" t="n"/>
+      <c r="B25" s="16" t="n"/>
       <c r="C25" s="33" t="n"/>
-      <c r="D25" s="16" t="n"/>
+      <c r="D25" s="33" t="n"/>
       <c r="E25" s="16" t="n"/>
       <c r="F25" s="16" t="n"/>
       <c r="G25" s="16" t="n"/>
@@ -11238,8 +11238,8 @@
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="B8:B16"/>
     <mergeCell ref="C8:C16"/>
-    <mergeCell ref="B17:B25"/>
     <mergeCell ref="C17:C25"/>
+    <mergeCell ref="D17:D25"/>
     <mergeCell ref="B26:B34"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="B35:B43"/>
@@ -11389,17 +11389,17 @@
       </c>
       <c r="F8" s="17" t="inlineStr">
         <is>
-          <t>TOL, TD/ G1, S3, M. Menad Abdallah</t>
+          <t>EDP, TD/ G1, S4, Mme Belmouhoub-Ould ali</t>
         </is>
       </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>EDP, TD/ G1, S2, Mme Belmouhoub-Ould ali</t>
+          <t>TRAL, TD/ G1, S2, M. Andasmas M</t>
         </is>
       </c>
       <c r="H8" s="17" t="inlineStr">
         <is>
-          <t>TRAL, TD/ G1, S15, M. Andasmas M</t>
+          <t>Géo. Diff, TD/ G1, S14, M. Fettouch Houari</t>
         </is>
       </c>
     </row>
@@ -11419,7 +11419,7 @@
       </c>
       <c r="F9" s="27" t="inlineStr">
         <is>
-          <t>EDP, TD/ G2, S4, Mme Belmouhoub-Ould ali</t>
+          <t>TOL, TD/ G2, S3, M. Menad Abdallah</t>
         </is>
       </c>
       <c r="G9" s="27" t="inlineStr">
@@ -11427,11 +11427,7 @@
           <t>TOL, TD/ G2, S15, M. Menad Abdallah</t>
         </is>
       </c>
-      <c r="H9" s="27" t="inlineStr">
-        <is>
-          <t>TOL, TD/ G2, S14, M. Menad Abdallah</t>
-        </is>
-      </c>
+      <c r="H9" s="27" t="n"/>
     </row>
     <row r="10" ht="21.75" customHeight="1" s="24">
       <c r="A10" s="30" t="n"/>
@@ -11509,24 +11505,24 @@
           <t>Lundi</t>
         </is>
       </c>
-      <c r="B17" s="29" t="inlineStr">
+      <c r="B17" s="17" t="inlineStr">
+        <is>
+          <t>TOL, TD/ G1, C4, M. Menad Abdallah</t>
+        </is>
+      </c>
+      <c r="C17" s="29" t="inlineStr">
+        <is>
+          <t>EDP, COUR/ section 1, Amphi3, Mme Belmouhoub-Ould ali</t>
+        </is>
+      </c>
+      <c r="D17" s="29" t="inlineStr">
         <is>
           <t>EDP, COUR/ section 1, Amphi2, Mme Belmouhoub-Ould ali</t>
         </is>
       </c>
-      <c r="C17" s="29" t="inlineStr">
-        <is>
-          <t>EDP, COUR/ section 1, Amphi3, Mme Belmouhoub-Ould ali</t>
-        </is>
-      </c>
-      <c r="D17" s="17" t="inlineStr">
-        <is>
-          <t>Géo. Diff, TD/ G1, C4, M. Fettouch Houari</t>
-        </is>
-      </c>
       <c r="E17" s="17" t="inlineStr">
         <is>
-          <t>Géo. Diff, TD/ G2, C1, M. Fettouch Houari</t>
+          <t>Géo. Diff, TD/ G2, B4, M. Fettouch Houari</t>
         </is>
       </c>
       <c r="F17" s="17" t="n"/>
@@ -11535,9 +11531,13 @@
     </row>
     <row r="18" ht="21.75" customHeight="1" s="24">
       <c r="A18" s="30" t="n"/>
-      <c r="B18" s="31" t="n"/>
+      <c r="B18" s="27" t="inlineStr">
+        <is>
+          <t>EDP, TD/ G2, S1, Mme Belmouhoub-Ould ali</t>
+        </is>
+      </c>
       <c r="C18" s="31" t="n"/>
-      <c r="D18" s="27" t="n"/>
+      <c r="D18" s="31" t="n"/>
       <c r="E18" s="27" t="n"/>
       <c r="F18" s="27" t="n"/>
       <c r="G18" s="27" t="n"/>
@@ -11545,9 +11545,9 @@
     </row>
     <row r="19" ht="21.75" customHeight="1" s="24">
       <c r="A19" s="30" t="n"/>
-      <c r="B19" s="31" t="n"/>
+      <c r="B19" s="27" t="n"/>
       <c r="C19" s="31" t="n"/>
-      <c r="D19" s="27" t="n"/>
+      <c r="D19" s="31" t="n"/>
       <c r="E19" s="27" t="n"/>
       <c r="F19" s="27" t="n"/>
       <c r="G19" s="27" t="n"/>
@@ -11555,9 +11555,9 @@
     </row>
     <row r="20" ht="21.75" customHeight="1" s="24">
       <c r="A20" s="30" t="n"/>
-      <c r="B20" s="31" t="n"/>
+      <c r="B20" s="27" t="n"/>
       <c r="C20" s="31" t="n"/>
-      <c r="D20" s="27" t="n"/>
+      <c r="D20" s="31" t="n"/>
       <c r="E20" s="27" t="n"/>
       <c r="F20" s="27" t="n"/>
       <c r="G20" s="27" t="n"/>
@@ -11565,9 +11565,9 @@
     </row>
     <row r="21" ht="21.75" customHeight="1" s="24">
       <c r="A21" s="30" t="n"/>
-      <c r="B21" s="31" t="n"/>
+      <c r="B21" s="27" t="n"/>
       <c r="C21" s="31" t="n"/>
-      <c r="D21" s="27" t="n"/>
+      <c r="D21" s="31" t="n"/>
       <c r="E21" s="27" t="n"/>
       <c r="F21" s="27" t="n"/>
       <c r="G21" s="27" t="n"/>
@@ -11575,9 +11575,9 @@
     </row>
     <row r="22" ht="21.75" customHeight="1" s="24">
       <c r="A22" s="30" t="n"/>
-      <c r="B22" s="31" t="n"/>
+      <c r="B22" s="27" t="n"/>
       <c r="C22" s="31" t="n"/>
-      <c r="D22" s="27" t="n"/>
+      <c r="D22" s="31" t="n"/>
       <c r="E22" s="27" t="n"/>
       <c r="F22" s="27" t="n"/>
       <c r="G22" s="27" t="n"/>
@@ -11585,9 +11585,9 @@
     </row>
     <row r="23" ht="21.75" customHeight="1" s="24">
       <c r="A23" s="30" t="n"/>
-      <c r="B23" s="31" t="n"/>
+      <c r="B23" s="27" t="n"/>
       <c r="C23" s="31" t="n"/>
-      <c r="D23" s="27" t="n"/>
+      <c r="D23" s="31" t="n"/>
       <c r="E23" s="27" t="n"/>
       <c r="F23" s="27" t="n"/>
       <c r="G23" s="27" t="n"/>
@@ -11595,9 +11595,9 @@
     </row>
     <row r="24" ht="21.75" customHeight="1" s="24">
       <c r="A24" s="30" t="n"/>
-      <c r="B24" s="31" t="n"/>
+      <c r="B24" s="27" t="n"/>
       <c r="C24" s="31" t="n"/>
-      <c r="D24" s="27" t="n"/>
+      <c r="D24" s="31" t="n"/>
       <c r="E24" s="27" t="n"/>
       <c r="F24" s="27" t="n"/>
       <c r="G24" s="27" t="n"/>
@@ -11605,9 +11605,9 @@
     </row>
     <row r="25" ht="21.75" customHeight="1" s="24">
       <c r="A25" s="32" t="n"/>
-      <c r="B25" s="33" t="n"/>
+      <c r="B25" s="16" t="n"/>
       <c r="C25" s="33" t="n"/>
-      <c r="D25" s="16" t="n"/>
+      <c r="D25" s="33" t="n"/>
       <c r="E25" s="16" t="n"/>
       <c r="F25" s="16" t="n"/>
       <c r="G25" s="16" t="n"/>
@@ -12897,8 +12897,8 @@
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="C8:C16"/>
     <mergeCell ref="D8:D16"/>
-    <mergeCell ref="B17:B25"/>
     <mergeCell ref="C17:C25"/>
+    <mergeCell ref="D17:D25"/>
     <mergeCell ref="B26:B34"/>
     <mergeCell ref="C26:C34"/>
     <mergeCell ref="B35:B43"/>
@@ -13162,7 +13162,7 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>SSI, COUR/ section 1, Amphi3, BENTAOUZA C</t>
+          <t>SSI, COUR/ section 1, Amphi2, BENTAOUZA C</t>
         </is>
       </c>
       <c r="C17" s="17" t="inlineStr">
@@ -13172,7 +13172,7 @@
       </c>
       <c r="D17" s="29" t="inlineStr">
         <is>
-          <t>OWS, COUR/ section 1, Amphi2, DJEBBARA R.</t>
+          <t>OWS, COUR/ section 1, Amphi3, DJEBBARA R.</t>
         </is>
       </c>
       <c r="E17" s="17" t="inlineStr">
@@ -14772,7 +14772,7 @@
       <c r="G8" s="17" t="n"/>
       <c r="H8" s="17" t="inlineStr">
         <is>
-          <t>AOSI, TD/ G1, S2, KHIAT</t>
+          <t>AOSI, TD/ G1, S15, KHIAT</t>
         </is>
       </c>
     </row>
@@ -14864,7 +14864,7 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>ASBDA, COUR/ section 1, C2, HABIB ZAHMANI M</t>
+          <t>ASBDA, COUR/ section 1, S12, HABIB ZAHMANI M</t>
         </is>
       </c>
       <c r="C17" s="29" t="inlineStr">
@@ -16414,7 +16414,7 @@
       </c>
       <c r="H8" s="17" t="inlineStr">
         <is>
-          <t>GéoDiff2, TD/ G1, S3, M. BELARBI Lakehal</t>
+          <t>GéoDiff2, TD/ G1, S2, M. BELARBI Lakehal</t>
         </is>
       </c>
     </row>
@@ -16506,7 +16506,7 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>GéoDiff2, COUR/ section 1, C3, M. BELARBI Lakehal</t>
+          <t>GéoDiff2, COUR/ section 1, S13, M. BELARBI Lakehal</t>
         </is>
       </c>
       <c r="C17" s="29" t="inlineStr">
@@ -16516,17 +16516,17 @@
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>Dis2, TD/ G1, S1, M. BOUZIT Hamid</t>
+          <t>Dis2, TD/ G1, C2, M. BOUZIT Hamid</t>
         </is>
       </c>
       <c r="E17" s="17" t="inlineStr">
         <is>
-          <t>EDP2, TD/ G1, C2, M. Andasmas M</t>
+          <t>EDP2, TD/ G1, C1, M. Andasmas M</t>
         </is>
       </c>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>EDP2, TD/ G1, S1, M. Andasmas M</t>
+          <t>EDP2, TD/ G1, S12, M. Andasmas M</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">

</xml_diff>